<commit_message>
disable salaries on excel
</commit_message>
<xml_diff>
--- a/public/excel/apl_form.xlsx
+++ b/public/excel/apl_form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INFOMINA\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Infomina\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -141,9 +141,6 @@
     <t>NOTICE PERIOD:____________________</t>
   </si>
   <si>
-    <t>INFOMINA SDN . BHD.(776590-U)</t>
-  </si>
-  <si>
     <t xml:space="preserve">  personal qualities or achievements not otherwise state in your resume.</t>
   </si>
   <si>
@@ -154,12 +151,15 @@
   </si>
   <si>
     <t>Refer to my resume from Recruitment Portal/Social Network _____________________________</t>
+  </si>
+  <si>
+    <t>INFOMINA BERHAD (776590-U)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -537,7 +537,7 @@
         <xdr:cNvPr id="3076" name="Rectangle 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000040C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000040C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -586,7 +586,7 @@
         <xdr:cNvPr id="3077" name="Rectangle 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000050C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000050C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -635,7 +635,7 @@
         <xdr:cNvPr id="3078" name="Rectangle 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000060C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000060C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1021,7 +1021,7 @@
   <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" colorId="22" zoomScale="87" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1038,7 +1038,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.45">
       <c r="A1" s="42" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1387,7 +1387,7 @@
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="41"/>
       <c r="B39" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39"/>
       <c r="D39"/>
@@ -1405,7 +1405,7 @@
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="41"/>
       <c r="B41" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41"/>
       <c r="D41"/>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I45" s="29"/>
     </row>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B53" s="37"/>
       <c r="C53" s="37"/>

</xml_diff>